<commit_message>
Apagar itens que não deveriam estar na aba de tamanho
</commit_message>
<xml_diff>
--- a/Documentacao_Especificacao/2023-12-17 - 1540 - Pablo Martins - Especificação endpoinst API atualizado, separar planilhas por rota.xlsx
+++ b/Documentacao_Especificacao/2023-12-17 - 1540 - Pablo Martins - Especificação endpoinst API atualizado, separar planilhas por rota.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TCC\Documentacao_Especificacao\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{594F897D-0E25-42B6-8CEF-B70E440CF92E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1555F83C-5256-446E-87B4-45DB5A2170B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{307990C6-2F35-404A-A571-FFC0C2848864}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{307990C6-2F35-404A-A571-FFC0C2848864}"/>
   </bookViews>
   <sheets>
     <sheet name="Endereço" sheetId="9" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="107">
   <si>
     <t>EndPoint</t>
   </si>
@@ -851,7 +851,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95DB7A6C-BD7B-40C5-8F8E-CCD565A6B65F}">
   <dimension ref="A1:J9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="94" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScale="94" workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -1040,10 +1040,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4BEEE4C-44BC-43F5-9BDA-674615679185}">
-  <dimension ref="A1:J16"/>
+  <dimension ref="A1:J9"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="66" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="66" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1208,224 +1208,21 @@
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:10" s="3" customFormat="1" ht="72" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="H6" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="I6" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" s="3" customFormat="1" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A7" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="H7" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="I7" s="3" t="s">
-        <v>33</v>
-      </c>
+    <row r="6" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="E6" s="4"/>
+      <c r="H6" s="4"/>
+    </row>
+    <row r="7" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="E7" s="4"/>
+      <c r="H7" s="4"/>
     </row>
     <row r="8" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="H8" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="I8" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" s="3" customFormat="1" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A9" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="H9" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="I9" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" s="3" customFormat="1" ht="172.8" x14ac:dyDescent="0.3">
-      <c r="A10" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="H10" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="I10" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" s="3" customFormat="1" ht="158.4" x14ac:dyDescent="0.3">
-      <c r="A11" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="F11" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="H11" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="I11" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="F12" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="G12" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="H12" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="I12" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="E13" s="4"/>
-      <c r="H13" s="4"/>
-    </row>
-    <row r="14" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="E14" s="4"/>
-      <c r="H14" s="4"/>
-    </row>
-    <row r="15" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="E15" s="4"/>
-      <c r="H15" s="4"/>
-    </row>
-    <row r="16" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="E16" s="4"/>
-      <c r="H16" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="H8" s="4"/>
+    </row>
+    <row r="9" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="E9" s="4"/>
+      <c r="H9" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>